<commit_message>
pathway and ppi added
</commit_message>
<xml_diff>
--- a/251120_CompHuman-SpatialJCI/Output_JCI/Conservation_Analysis/Conservation_Analysis.xlsx
+++ b/251120_CompHuman-SpatialJCI/Output_JCI/Conservation_Analysis/Conservation_Analysis.xlsx
@@ -8,13 +8,15 @@
   <sheets>
     <sheet name="Conservation_Stats" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="HighConserved_mySC" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="HighConserved_majorSC" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="HighConserved_ImmSC" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="HighConserved_majorSC" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="HighConserved_aggSC" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t xml:space="preserve">comparison</t>
   </si>
@@ -70,6 +72,9 @@
     <t xml:space="preserve">majorSC</t>
   </si>
   <si>
+    <t xml:space="preserve">aggSC</t>
+  </si>
+  <si>
     <t xml:space="preserve">DRvsHFD</t>
   </si>
   <si>
@@ -94,7 +99,43 @@
     <t xml:space="preserve">HFDvsSD, DRvsHFD, EXvsHFD</t>
   </si>
   <si>
+    <t xml:space="preserve">Fgf1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chst2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HFDvsSD, DRvsHFD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mbp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HFDvsSD, EXvsHFD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HFDvsSD, DRvsHFD, DREXvsHFD</t>
+  </si>
+  <si>
     <t xml:space="preserve">DRvsHFD, EXvsHFD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fam107a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mlip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Egr2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXvsHFD, DREXvsHFD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gpm6a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pmp2</t>
   </si>
 </sst>
 </file>
@@ -475,7 +516,7 @@
         <v>14</v>
       </c>
       <c r="C2" t="n">
-        <v>27</v>
+        <v>510</v>
       </c>
       <c r="D2" t="n">
         <v>194</v>
@@ -484,28 +525,28 @@
         <v>1422</v>
       </c>
       <c r="F2" t="n">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="G2" t="n">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="H2" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I2" t="n">
-        <v>22</v>
+        <v>463</v>
       </c>
       <c r="J2" t="n">
-        <v>0.0740740740740741</v>
+        <v>0.0274509803921569</v>
       </c>
       <c r="K2" t="n">
-        <v>0.148148148148148</v>
+        <v>0.0745098039215686</v>
       </c>
       <c r="L2" t="n">
-        <v>0.185185185185185</v>
+        <v>0.092156862745098</v>
       </c>
       <c r="M2" t="n">
-        <v>0.037037037037037</v>
+        <v>0.00980392156862745</v>
       </c>
     </row>
     <row r="3">
@@ -516,7 +557,7 @@
         <v>15</v>
       </c>
       <c r="C3" t="n">
-        <v>4</v>
+        <v>215</v>
       </c>
       <c r="D3" t="n">
         <v>194</v>
@@ -525,25 +566,25 @@
         <v>1422</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G3" t="n">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>3</v>
+        <v>192</v>
       </c>
       <c r="J3" t="n">
-        <v>0</v>
+        <v>0.0232558139534884</v>
       </c>
       <c r="K3" t="n">
-        <v>0.25</v>
+        <v>0.0837209302325581</v>
       </c>
       <c r="L3" t="n">
-        <v>0.25</v>
+        <v>0.106976744186047</v>
       </c>
       <c r="M3" t="n">
         <v>0</v>
@@ -557,7 +598,7 @@
         <v>16</v>
       </c>
       <c r="C4" t="n">
-        <v>3</v>
+        <v>138</v>
       </c>
       <c r="D4" t="n">
         <v>194</v>
@@ -566,28 +607,28 @@
         <v>1422</v>
       </c>
       <c r="F4" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G4" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="H4" t="n">
         <v>1</v>
       </c>
       <c r="I4" t="n">
-        <v>2</v>
+        <v>123</v>
       </c>
       <c r="J4" t="n">
-        <v>0.333333333333333</v>
+        <v>0.0289855072463768</v>
       </c>
       <c r="K4" t="n">
-        <v>0.333333333333333</v>
+        <v>0.0869565217391304</v>
       </c>
       <c r="L4" t="n">
-        <v>0.333333333333333</v>
+        <v>0.108695652173913</v>
       </c>
       <c r="M4" t="n">
-        <v>0.333333333333333</v>
+        <v>0.0072463768115942</v>
       </c>
     </row>
     <row r="5">
@@ -598,7 +639,7 @@
         <v>17</v>
       </c>
       <c r="C5" t="n">
-        <v>69</v>
+        <v>416</v>
       </c>
       <c r="D5" t="n">
         <v>194</v>
@@ -607,39 +648,39 @@
         <v>1422</v>
       </c>
       <c r="F5" t="n">
+        <v>13</v>
+      </c>
+      <c r="G5" t="n">
+        <v>37</v>
+      </c>
+      <c r="H5" t="n">
         <v>5</v>
       </c>
-      <c r="G5" t="n">
-        <v>11</v>
-      </c>
-      <c r="H5" t="n">
-        <v>1</v>
-      </c>
       <c r="I5" t="n">
-        <v>54</v>
+        <v>371</v>
       </c>
       <c r="J5" t="n">
-        <v>0.072463768115942</v>
+        <v>0.03125</v>
       </c>
       <c r="K5" t="n">
-        <v>0.159420289855072</v>
+        <v>0.0889423076923077</v>
       </c>
       <c r="L5" t="n">
-        <v>0.217391304347826</v>
+        <v>0.108173076923077</v>
       </c>
       <c r="M5" t="n">
-        <v>0.0144927536231884</v>
+        <v>0.0120192307692308</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
         <v>18</v>
       </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
       <c r="C6" t="n">
-        <v>47</v>
+        <v>806</v>
       </c>
       <c r="D6" t="n">
         <v>194</v>
@@ -648,39 +689,39 @@
         <v>1422</v>
       </c>
       <c r="F6" t="n">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="G6" t="n">
-        <v>9</v>
+        <v>62</v>
       </c>
       <c r="H6" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I6" t="n">
-        <v>37</v>
+        <v>728</v>
       </c>
       <c r="J6" t="n">
-        <v>0.0638297872340425</v>
+        <v>0.0260545905707196</v>
       </c>
       <c r="K6" t="n">
-        <v>0.191489361702128</v>
+        <v>0.0769230769230769</v>
       </c>
       <c r="L6" t="n">
-        <v>0.212765957446809</v>
+        <v>0.0967741935483871</v>
       </c>
       <c r="M6" t="n">
-        <v>0.0425531914893617</v>
+        <v>0.00620347394540943</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>5</v>
+        <v>770</v>
       </c>
       <c r="D7" t="n">
         <v>194</v>
@@ -689,39 +730,39 @@
         <v>1422</v>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G7" t="n">
-        <v>2</v>
+        <v>67</v>
       </c>
       <c r="H7" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I7" t="n">
-        <v>3</v>
+        <v>693</v>
       </c>
       <c r="J7" t="n">
-        <v>0</v>
+        <v>0.0207792207792208</v>
       </c>
       <c r="K7" t="n">
-        <v>0.4</v>
+        <v>0.087012987012987</v>
       </c>
       <c r="L7" t="n">
-        <v>0.4</v>
+        <v>0.1</v>
       </c>
       <c r="M7" t="n">
-        <v>0</v>
+        <v>0.00779220779220779</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C8" t="n">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="D8" t="n">
         <v>194</v>
@@ -730,28 +771,28 @@
         <v>1422</v>
       </c>
       <c r="F8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G8" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I8" t="n">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="J8" t="n">
-        <v>0.0181818181818182</v>
+        <v>0.0303030303030303</v>
       </c>
       <c r="K8" t="n">
-        <v>0.218181818181818</v>
+        <v>0.151515151515152</v>
       </c>
       <c r="L8" t="n">
-        <v>0.218181818181818</v>
+        <v>0.181818181818182</v>
       </c>
       <c r="M8" t="n">
-        <v>0.0181818181818182</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -759,10 +800,10 @@
         <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C9" t="n">
-        <v>186</v>
+        <v>114</v>
       </c>
       <c r="D9" t="n">
         <v>194</v>
@@ -771,28 +812,28 @@
         <v>1422</v>
       </c>
       <c r="F9" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" t="n">
         <v>5</v>
       </c>
-      <c r="G9" t="n">
-        <v>29</v>
-      </c>
       <c r="H9" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>154</v>
+        <v>108</v>
       </c>
       <c r="J9" t="n">
-        <v>0.0268817204301075</v>
+        <v>0.0087719298245614</v>
       </c>
       <c r="K9" t="n">
-        <v>0.155913978494624</v>
+        <v>0.043859649122807</v>
       </c>
       <c r="L9" t="n">
-        <v>0.172043010752688</v>
+        <v>0.0526315789473684</v>
       </c>
       <c r="M9" t="n">
-        <v>0.010752688172043</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -800,10 +841,10 @@
         <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C10" t="n">
-        <v>3</v>
+        <v>825</v>
       </c>
       <c r="D10" t="n">
         <v>194</v>
@@ -812,28 +853,28 @@
         <v>1422</v>
       </c>
       <c r="F10" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="G10" t="n">
-        <v>0</v>
+        <v>71</v>
       </c>
       <c r="H10" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I10" t="n">
-        <v>3</v>
+        <v>742</v>
       </c>
       <c r="J10" t="n">
-        <v>0</v>
+        <v>0.0206060606060606</v>
       </c>
       <c r="K10" t="n">
-        <v>0</v>
+        <v>0.0860606060606061</v>
       </c>
       <c r="L10" t="n">
-        <v>0</v>
+        <v>0.100606060606061</v>
       </c>
       <c r="M10" t="n">
-        <v>0</v>
+        <v>0.00606060606060606</v>
       </c>
     </row>
     <row r="11">
@@ -841,10 +882,10 @@
         <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C11" t="n">
-        <v>10</v>
+        <v>919</v>
       </c>
       <c r="D11" t="n">
         <v>194</v>
@@ -853,39 +894,39 @@
         <v>1422</v>
       </c>
       <c r="F11" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="G11" t="n">
-        <v>3</v>
+        <v>76</v>
       </c>
       <c r="H11" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I11" t="n">
-        <v>7</v>
+        <v>830</v>
       </c>
       <c r="J11" t="n">
-        <v>0</v>
+        <v>0.0206746463547334</v>
       </c>
       <c r="K11" t="n">
-        <v>0.3</v>
+        <v>0.0826985854189336</v>
       </c>
       <c r="L11" t="n">
-        <v>0.3</v>
+        <v>0.0968443960826986</v>
       </c>
       <c r="M11" t="n">
-        <v>0</v>
+        <v>0.00652883569096844</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C12" t="n">
-        <v>537</v>
+        <v>1337</v>
       </c>
       <c r="D12" t="n">
         <v>194</v>
@@ -894,28 +935,28 @@
         <v>1422</v>
       </c>
       <c r="F12" t="n">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="G12" t="n">
-        <v>52</v>
+        <v>105</v>
       </c>
       <c r="H12" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I12" t="n">
-        <v>476</v>
+        <v>1217</v>
       </c>
       <c r="J12" t="n">
-        <v>0.0242085661080074</v>
+        <v>0.0134629768137622</v>
       </c>
       <c r="K12" t="n">
-        <v>0.0968342644320298</v>
+        <v>0.0785340314136126</v>
       </c>
       <c r="L12" t="n">
-        <v>0.113594040968343</v>
+        <v>0.0897531787584144</v>
       </c>
       <c r="M12" t="n">
-        <v>0.0074487895716946</v>
+        <v>0.00224382946896036</v>
       </c>
     </row>
     <row r="13">
@@ -923,10 +964,10 @@
         <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C13" t="n">
-        <v>90</v>
+        <v>242</v>
       </c>
       <c r="D13" t="n">
         <v>194</v>
@@ -935,25 +976,25 @@
         <v>1422</v>
       </c>
       <c r="F13" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G13" t="n">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="H13" t="n">
         <v>0</v>
       </c>
       <c r="I13" t="n">
-        <v>73</v>
+        <v>215</v>
       </c>
       <c r="J13" t="n">
-        <v>0.0222222222222222</v>
+        <v>0.00413223140495868</v>
       </c>
       <c r="K13" t="n">
-        <v>0.166666666666667</v>
+        <v>0.107438016528926</v>
       </c>
       <c r="L13" t="n">
-        <v>0.188888888888889</v>
+        <v>0.111570247933884</v>
       </c>
       <c r="M13" t="n">
         <v>0</v>
@@ -964,10 +1005,10 @@
         <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C14" t="n">
-        <v>19</v>
+        <v>240</v>
       </c>
       <c r="D14" t="n">
         <v>194</v>
@@ -976,28 +1017,28 @@
         <v>1422</v>
       </c>
       <c r="F14" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G14" t="n">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="H14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I14" t="n">
-        <v>17</v>
+        <v>216</v>
       </c>
       <c r="J14" t="n">
-        <v>0</v>
+        <v>0.0166666666666667</v>
       </c>
       <c r="K14" t="n">
-        <v>0.105263157894737</v>
+        <v>0.0875</v>
       </c>
       <c r="L14" t="n">
-        <v>0.105263157894737</v>
+        <v>0.1</v>
       </c>
       <c r="M14" t="n">
-        <v>0</v>
+        <v>0.00416666666666667</v>
       </c>
     </row>
     <row r="15">
@@ -1005,10 +1046,10 @@
         <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C15" t="n">
-        <v>26</v>
+        <v>2371</v>
       </c>
       <c r="D15" t="n">
         <v>194</v>
@@ -1017,28 +1058,28 @@
         <v>1422</v>
       </c>
       <c r="F15" t="n">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="G15" t="n">
-        <v>5</v>
+        <v>169</v>
       </c>
       <c r="H15" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="I15" t="n">
-        <v>21</v>
+        <v>2176</v>
       </c>
       <c r="J15" t="n">
-        <v>0</v>
+        <v>0.0156052298608182</v>
       </c>
       <c r="K15" t="n">
-        <v>0.192307692307692</v>
+        <v>0.0712779417967103</v>
       </c>
       <c r="L15" t="n">
-        <v>0.192307692307692</v>
+        <v>0.0822437789962041</v>
       </c>
       <c r="M15" t="n">
-        <v>0</v>
+        <v>0.00463939266132434</v>
       </c>
     </row>
     <row r="16">
@@ -1046,40 +1087,245 @@
         <v>20</v>
       </c>
       <c r="B16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" t="n">
+        <v>1600</v>
+      </c>
+      <c r="D16" t="n">
+        <v>194</v>
+      </c>
+      <c r="E16" t="n">
+        <v>1422</v>
+      </c>
+      <c r="F16" t="n">
+        <v>20</v>
+      </c>
+      <c r="G16" t="n">
+        <v>130</v>
+      </c>
+      <c r="H16" t="n">
+        <v>3</v>
+      </c>
+      <c r="I16" t="n">
+        <v>1453</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0.0125</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0.08125</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0.091875</v>
+      </c>
+      <c r="M16" t="n">
+        <v>0.001875</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" t="n">
+        <v>529</v>
+      </c>
+      <c r="D17" t="n">
+        <v>194</v>
+      </c>
+      <c r="E17" t="n">
+        <v>1422</v>
+      </c>
+      <c r="F17" t="n">
+        <v>11</v>
+      </c>
+      <c r="G17" t="n">
+        <v>47</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0</v>
+      </c>
+      <c r="I17" t="n">
+        <v>471</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0.0207939508506616</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0.0888468809073724</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0.109640831758034</v>
+      </c>
+      <c r="M17" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" t="n">
+        <v>238</v>
+      </c>
+      <c r="D18" t="n">
+        <v>194</v>
+      </c>
+      <c r="E18" t="n">
+        <v>1422</v>
+      </c>
+      <c r="F18" t="n">
+        <v>10</v>
+      </c>
+      <c r="G18" t="n">
+        <v>22</v>
+      </c>
+      <c r="H18" t="n">
+        <v>1</v>
+      </c>
+      <c r="I18" t="n">
+        <v>207</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0.0420168067226891</v>
+      </c>
+      <c r="K18" t="n">
+        <v>0.092436974789916</v>
+      </c>
+      <c r="L18" t="n">
+        <v>0.130252100840336</v>
+      </c>
+      <c r="M18" t="n">
+        <v>0.00420168067226891</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" t="n">
+        <v>444</v>
+      </c>
+      <c r="D19" t="n">
+        <v>194</v>
+      </c>
+      <c r="E19" t="n">
+        <v>1422</v>
+      </c>
+      <c r="F19" t="n">
+        <v>6</v>
+      </c>
+      <c r="G19" t="n">
+        <v>48</v>
+      </c>
+      <c r="H19" t="n">
+        <v>1</v>
+      </c>
+      <c r="I19" t="n">
+        <v>391</v>
+      </c>
+      <c r="J19" t="n">
+        <v>0.0135135135135135</v>
+      </c>
+      <c r="K19" t="n">
+        <v>0.108108108108108</v>
+      </c>
+      <c r="L19" t="n">
+        <v>0.119369369369369</v>
+      </c>
+      <c r="M19" t="n">
+        <v>0.00225225225225225</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" t="s">
         <v>17</v>
       </c>
-      <c r="C16" t="n">
-        <v>164</v>
-      </c>
-      <c r="D16" t="n">
-        <v>194</v>
-      </c>
-      <c r="E16" t="n">
-        <v>1422</v>
-      </c>
-      <c r="F16" t="n">
-        <v>2</v>
-      </c>
-      <c r="G16" t="n">
-        <v>26</v>
-      </c>
-      <c r="H16" t="n">
-        <v>0</v>
-      </c>
-      <c r="I16" t="n">
-        <v>136</v>
-      </c>
-      <c r="J16" t="n">
-        <v>0.0121951219512195</v>
-      </c>
-      <c r="K16" t="n">
-        <v>0.158536585365854</v>
-      </c>
-      <c r="L16" t="n">
-        <v>0.170731707317073</v>
-      </c>
-      <c r="M16" t="n">
-        <v>0</v>
+      <c r="C20" t="n">
+        <v>1023</v>
+      </c>
+      <c r="D20" t="n">
+        <v>194</v>
+      </c>
+      <c r="E20" t="n">
+        <v>1422</v>
+      </c>
+      <c r="F20" t="n">
+        <v>16</v>
+      </c>
+      <c r="G20" t="n">
+        <v>81</v>
+      </c>
+      <c r="H20" t="n">
+        <v>4</v>
+      </c>
+      <c r="I20" t="n">
+        <v>930</v>
+      </c>
+      <c r="J20" t="n">
+        <v>0.0156402737047898</v>
+      </c>
+      <c r="K20" t="n">
+        <v>0.0791788856304985</v>
+      </c>
+      <c r="L20" t="n">
+        <v>0.0909090909090909</v>
+      </c>
+      <c r="M20" t="n">
+        <v>0.00391006842619746</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" t="n">
+        <v>1006</v>
+      </c>
+      <c r="D21" t="n">
+        <v>194</v>
+      </c>
+      <c r="E21" t="n">
+        <v>1422</v>
+      </c>
+      <c r="F21" t="n">
+        <v>21</v>
+      </c>
+      <c r="G21" t="n">
+        <v>90</v>
+      </c>
+      <c r="H21" t="n">
+        <v>1</v>
+      </c>
+      <c r="I21" t="n">
+        <v>896</v>
+      </c>
+      <c r="J21" t="n">
+        <v>0.0208747514910537</v>
+      </c>
+      <c r="K21" t="n">
+        <v>0.0894632206759443</v>
+      </c>
+      <c r="L21" t="n">
+        <v>0.10934393638171</v>
+      </c>
+      <c r="M21" t="n">
+        <v>0.00099403578528827</v>
       </c>
     </row>
   </sheetData>
@@ -1098,24 +1344,57 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B2" t="n">
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="n">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" t="n">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1134,24 +1413,206 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B2" t="n">
         <v>2</v>
       </c>
       <c r="C2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" t="n">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" t="n">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" t="n">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" t="n">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" t="n">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" t="n">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="n">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="n">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>